<commit_message>
Sat Sep  4 19:17:14 CST 2021
</commit_message>
<xml_diff>
--- a/笔记/CISA/CISA知识点.xlsx
+++ b/笔记/CISA/CISA知识点.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21600" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="13180" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="学习计划" sheetId="7" r:id="rId1"/>
@@ -18706,10 +18706,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -18775,26 +18775,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -18805,8 +18790,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -18829,6 +18828,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -18836,53 +18843,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -18904,16 +18867,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -19019,13 +19019,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19043,19 +19043,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19073,19 +19091,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19097,7 +19127,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19115,13 +19157,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19133,7 +19175,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19145,61 +19187,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19377,26 +19377,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -19412,17 +19392,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -19444,9 +19418,35 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -19455,148 +19455,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -27756,7 +27756,7 @@
   <sheetPr/>
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -34581,8 +34581,8 @@
   <sheetPr/>
   <dimension ref="A1:E129"/>
   <sheetViews>
-    <sheetView zoomScale="99" zoomScaleNormal="99" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:B25"/>
+    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="4"/>
@@ -36305,9 +36305,9 @@
   <dimension ref="A1:E259"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A195" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19:B20"/>
+      <selection pane="bottomLeft" activeCell="C197" sqref="C197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="4"/>
@@ -39511,10 +39511,10 @@
   <sheetPr/>
   <dimension ref="A1:E347"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A298" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C104" sqref="C104"/>
+      <selection pane="bottomLeft" activeCell="C306" sqref="C306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="4"/>

</xml_diff>

<commit_message>
Tue Nov  2 11:21:18 CST 2021
</commit_message>
<xml_diff>
--- a/笔记/CISA/CISA知识点.xlsx
+++ b/笔记/CISA/CISA知识点.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13180" activeTab="4"/>
+    <workbookView windowWidth="28800" windowHeight="13180" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="学习计划" sheetId="7" r:id="rId1"/>
@@ -18706,9 +18706,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="34">
@@ -18783,24 +18783,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -18812,79 +18807,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -18913,7 +18837,83 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -19019,7 +19019,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19037,43 +19157,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19085,7 +19181,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19097,109 +19199,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19353,26 +19353,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -19392,11 +19392,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -19427,17 +19433,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -19455,142 +19455,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -31812,9 +31812,9 @@
   <dimension ref="A1:E221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C56" sqref="C56:D56"/>
+      <selection pane="bottomLeft" activeCell="C189" sqref="C189:D189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="4"/>
@@ -34581,7 +34581,7 @@
   <sheetPr/>
   <dimension ref="A1:E129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" topLeftCell="A85" workbookViewId="0">
+    <sheetView zoomScale="99" zoomScaleNormal="99" topLeftCell="A114" workbookViewId="0">
       <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
@@ -36304,10 +36304,10 @@
   <sheetPr/>
   <dimension ref="A1:E259"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A195" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C197" sqref="C197"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="4"/>
@@ -39511,8 +39511,8 @@
   <sheetPr/>
   <dimension ref="A1:E347"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A298" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A323" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="C306" sqref="C306"/>
     </sheetView>

</xml_diff>

<commit_message>
Sat Dec 11 18:23:42 CST 2021
</commit_message>
<xml_diff>
--- a/笔记/CISA/CISA知识点.xlsx
+++ b/笔记/CISA/CISA知识点.xlsx
@@ -18706,9 +18706,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="34">
@@ -18777,33 +18777,9 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -18814,18 +18790,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -18837,15 +18813,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -18853,6 +18836,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -18874,22 +18865,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -18897,23 +18872,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -19019,31 +19019,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19055,13 +19037,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19079,25 +19055,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19115,85 +19181,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19353,17 +19353,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -19371,23 +19365,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -19403,6 +19382,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -19437,16 +19431,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -19455,148 +19455,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -36305,9 +36305,9 @@
   <dimension ref="A1:E259"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="C171" sqref="C171:C173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="4"/>

</xml_diff>

<commit_message>
Thu Jul 28 14:50:59 CST 2022
</commit_message>
<xml_diff>
--- a/笔记/CISA/CISA知识点.xlsx
+++ b/笔记/CISA/CISA知识点.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13180" activeTab="5"/>
+    <workbookView windowWidth="28000" windowHeight="12840" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="学习计划" sheetId="7" r:id="rId1"/>
@@ -18706,10 +18706,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -18777,7 +18777,14 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -18792,6 +18799,92 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -18799,14 +18892,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -18826,94 +18912,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -19019,19 +19019,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19049,13 +19055,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19067,7 +19097,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19079,7 +19127,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19091,7 +19187,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19103,103 +19199,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19353,11 +19353,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -19365,8 +19371,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -19386,17 +19401,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -19430,23 +19445,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -19455,148 +19455,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -27757,7 +27757,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="38.6640625" defaultRowHeight="40" customHeight="1" outlineLevelCol="3"/>
@@ -28247,9 +28247,9 @@
   <dimension ref="A1:E295"/>
   <sheetViews>
     <sheetView zoomScale="101" zoomScaleNormal="101" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C138" sqref="C138:D138"/>
+      <selection pane="bottomLeft" activeCell="D126" sqref="D126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="4"/>
@@ -31812,9 +31812,9 @@
   <dimension ref="A1:E221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C189" sqref="C189:D189"/>
+      <selection pane="bottomLeft" activeCell="C201" sqref="C201:D201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="4"/>
@@ -36304,10 +36304,10 @@
   <sheetPr/>
   <dimension ref="A1:E259"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A199" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C171" sqref="C171:C173"/>
+      <selection pane="bottomLeft" activeCell="A210" sqref="A210:A222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="4"/>
@@ -39511,10 +39511,10 @@
   <sheetPr/>
   <dimension ref="A1:E347"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A323" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C306" sqref="C306"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45:D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="4"/>

</xml_diff>

<commit_message>
Wed Sep 13 20:26:18 CST 2023
</commit_message>
<xml_diff>
--- a/笔记/CISA/CISA知识点.xlsx
+++ b/笔记/CISA/CISA知识点.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="12840" activeTab="6"/>
+    <workbookView windowHeight="16820" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="学习计划" sheetId="7" r:id="rId1"/>
@@ -329,7 +329,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4102" uniqueCount="3159">
   <si>
     <t>核查单</t>
   </si>
@@ -12941,13 +12941,26 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>宣告灾难的程序（上报程序）</t>
+    </r>
+    <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">1. </t>
+      <t xml:space="preserve">
+2.</t>
     </r>
     <r>
       <rPr>
@@ -12956,26 +12969,16 @@
         <rFont val="Calibri"/>
         <charset val="134"/>
       </rPr>
-      <t>宣告灾难的程序（上报程序）</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-2.</t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> 启用计划的条件（什么条件启用它）</t>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>启用计划的条件（什么条件启用它）</t>
     </r>
     <r>
       <rPr>
@@ -18706,12 +18709,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="34">
+  <fonts count="36">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -18798,34 +18801,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -18840,6 +18819,59 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -18860,8 +18892,15 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -18877,43 +18916,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -18954,6 +18957,17 @@
       <color rgb="FFC00000"/>
       <name val="宋体"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
     </font>
   </fonts>
   <fills count="42">
@@ -19019,121 +19033,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19145,25 +19045,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19181,7 +19069,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19193,13 +19207,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -19353,21 +19367,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -19450,147 +19449,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="40" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -20033,6 +20047,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -20109,9 +20126,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -20603,7 +20617,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:C24"/>
   <sheetViews>
@@ -20815,7 +20829,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:B95"/>
   <sheetViews>
@@ -21429,7 +21443,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:W287"/>
   <sheetViews>
@@ -27752,7 +27766,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:D49"/>
   <sheetViews>
@@ -28242,12 +28256,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:E295"/>
   <sheetViews>
     <sheetView zoomScale="101" zoomScaleNormal="101" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="D126" sqref="D126"/>
     </sheetView>
@@ -28256,7 +28270,7 @@
   <cols>
     <col min="1" max="1" width="15.234375" style="106" customWidth="1"/>
     <col min="2" max="3" width="25.625" style="37" customWidth="1"/>
-    <col min="4" max="4" width="88.4140625" style="161" customWidth="1"/>
+    <col min="4" max="4" width="88.4140625" style="162" customWidth="1"/>
     <col min="5" max="5" width="64.9765625" style="37" customWidth="1"/>
     <col min="6" max="16384" width="9" style="37"/>
   </cols>
@@ -28268,10 +28282,10 @@
       <c r="B1" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="152" t="s">
+      <c r="C1" s="153" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="162"/>
+      <c r="D1" s="163"/>
       <c r="E1" s="24" t="s">
         <v>101</v>
       </c>
@@ -28292,10 +28306,10 @@
     <row r="3" customHeight="1" spans="1:5">
       <c r="A3" s="107"/>
       <c r="B3" s="42"/>
-      <c r="C3" s="163" t="s">
+      <c r="C3" s="164" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="164"/>
+      <c r="D3" s="165"/>
       <c r="E3" s="49"/>
     </row>
     <row r="4" ht="120" customHeight="1" spans="1:5">
@@ -28314,10 +28328,10 @@
       <c r="B5" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="165" t="s">
+      <c r="C5" s="166" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="166"/>
+      <c r="D5" s="167"/>
       <c r="E5" s="49"/>
     </row>
     <row r="6" customHeight="1" spans="1:5">
@@ -28325,10 +28339,10 @@
       <c r="B6" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="167" t="s">
+      <c r="C6" s="168" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="167"/>
+      <c r="D6" s="168"/>
       <c r="E6" s="44" t="s">
         <v>111</v>
       </c>
@@ -28336,28 +28350,28 @@
     <row r="7" customHeight="1" spans="1:5">
       <c r="A7" s="107"/>
       <c r="B7" s="49"/>
-      <c r="C7" s="167" t="s">
+      <c r="C7" s="168" t="s">
         <v>112</v>
       </c>
-      <c r="D7" s="167"/>
+      <c r="D7" s="168"/>
       <c r="E7" s="40"/>
     </row>
     <row r="8" customHeight="1" spans="1:5">
       <c r="A8" s="107"/>
       <c r="B8" s="49"/>
-      <c r="C8" s="167" t="s">
+      <c r="C8" s="168" t="s">
         <v>113</v>
       </c>
-      <c r="D8" s="167"/>
+      <c r="D8" s="168"/>
       <c r="E8" s="40"/>
     </row>
     <row r="9" customHeight="1" spans="1:5">
       <c r="A9" s="107"/>
       <c r="B9" s="49"/>
-      <c r="C9" s="167" t="s">
+      <c r="C9" s="168" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="167"/>
+      <c r="D9" s="168"/>
       <c r="E9" s="42"/>
     </row>
     <row r="10" customHeight="1" spans="1:5">
@@ -28370,7 +28384,7 @@
       <c r="C10" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="D10" s="168" t="s">
+      <c r="D10" s="169" t="s">
         <v>118</v>
       </c>
       <c r="E10" s="49"/>
@@ -28379,7 +28393,7 @@
       <c r="A11" s="112"/>
       <c r="B11" s="40"/>
       <c r="C11" s="40"/>
-      <c r="D11" s="169" t="s">
+      <c r="D11" s="170" t="s">
         <v>119</v>
       </c>
       <c r="E11" s="49"/>
@@ -28542,7 +28556,7 @@
       <c r="C26" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="D26" s="170" t="s">
+      <c r="D26" s="144" t="s">
         <v>147</v>
       </c>
       <c r="E26" s="49"/>
@@ -28571,7 +28585,7 @@
       <c r="C29" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="D29" s="148"/>
+      <c r="D29" s="149"/>
       <c r="E29" s="49"/>
     </row>
     <row r="30" customHeight="1" spans="1:5">
@@ -28580,7 +28594,7 @@
       <c r="C30" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D30" s="148"/>
+      <c r="D30" s="149"/>
       <c r="E30" s="49"/>
     </row>
     <row r="31" customHeight="1" spans="1:5">
@@ -28589,7 +28603,7 @@
       <c r="C31" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="D31" s="148"/>
+      <c r="D31" s="149"/>
       <c r="E31" s="49"/>
     </row>
     <row r="32" ht="58" customHeight="1" spans="1:5">
@@ -28790,7 +28804,7 @@
       <c r="C50" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="D50" s="148"/>
+      <c r="D50" s="149"/>
       <c r="E50" s="49" t="s">
         <v>187</v>
       </c>
@@ -28801,7 +28815,7 @@
       <c r="C51" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="D51" s="148"/>
+      <c r="D51" s="149"/>
       <c r="E51" s="49" t="s">
         <v>189</v>
       </c>
@@ -31807,12 +31821,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:E221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="C201" sqref="C201:D201"/>
     </sheetView>
@@ -31834,10 +31848,10 @@
       <c r="B1" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="152" t="s">
+      <c r="C1" s="153" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="153"/>
+      <c r="D1" s="154"/>
       <c r="E1" s="24" t="s">
         <v>101</v>
       </c>
@@ -32685,23 +32699,23 @@
       <c r="A75" s="110" t="s">
         <v>830</v>
       </c>
-      <c r="B75" s="154" t="s">
+      <c r="B75" s="155" t="s">
         <v>831</v>
       </c>
-      <c r="C75" s="155" t="s">
+      <c r="C75" s="156" t="s">
         <v>832</v>
       </c>
-      <c r="D75" s="156"/>
-      <c r="E75" s="154"/>
+      <c r="D75" s="157"/>
+      <c r="E75" s="155"/>
     </row>
     <row r="76" customHeight="1" spans="1:5">
       <c r="A76" s="112"/>
-      <c r="B76" s="157"/>
-      <c r="C76" s="155" t="s">
+      <c r="B76" s="158"/>
+      <c r="C76" s="156" t="s">
         <v>833</v>
       </c>
-      <c r="D76" s="156"/>
-      <c r="E76" s="157"/>
+      <c r="D76" s="157"/>
+      <c r="E76" s="158"/>
     </row>
     <row r="77" ht="101" customHeight="1" spans="1:5">
       <c r="A77" s="112"/>
@@ -32953,7 +32967,7 @@
       <c r="B98" s="44" t="s">
         <v>881</v>
       </c>
-      <c r="C98" s="150" t="s">
+      <c r="C98" s="151" t="s">
         <v>882</v>
       </c>
       <c r="D98" s="143"/>
@@ -32978,7 +32992,7 @@
       <c r="C100" s="49" t="s">
         <v>885</v>
       </c>
-      <c r="D100" s="148" t="s">
+      <c r="D100" s="149" t="s">
         <v>886</v>
       </c>
       <c r="E100" s="49"/>
@@ -33323,7 +33337,7 @@
       <c r="B132" s="44" t="s">
         <v>943</v>
       </c>
-      <c r="C132" s="158" t="s">
+      <c r="C132" s="159" t="s">
         <v>944</v>
       </c>
       <c r="D132" s="11" t="s">
@@ -33334,7 +33348,7 @@
     <row r="133" customHeight="1" spans="1:5">
       <c r="A133" s="112"/>
       <c r="B133" s="40"/>
-      <c r="C133" s="159"/>
+      <c r="C133" s="160"/>
       <c r="D133" s="11" t="s">
         <v>946</v>
       </c>
@@ -33343,7 +33357,7 @@
     <row r="134" customHeight="1" spans="1:5">
       <c r="A134" s="112"/>
       <c r="B134" s="40"/>
-      <c r="C134" s="159"/>
+      <c r="C134" s="160"/>
       <c r="D134" s="11" t="s">
         <v>947</v>
       </c>
@@ -33352,7 +33366,7 @@
     <row r="135" customHeight="1" spans="1:5">
       <c r="A135" s="112"/>
       <c r="B135" s="40"/>
-      <c r="C135" s="160"/>
+      <c r="C135" s="161"/>
       <c r="D135" s="49" t="s">
         <v>948</v>
       </c>
@@ -33361,7 +33375,7 @@
     <row r="136" customHeight="1" spans="1:5">
       <c r="A136" s="112"/>
       <c r="B136" s="40"/>
-      <c r="C136" s="158" t="s">
+      <c r="C136" s="159" t="s">
         <v>949</v>
       </c>
       <c r="D136" s="11" t="s">
@@ -33372,7 +33386,7 @@
     <row r="137" customHeight="1" spans="1:5">
       <c r="A137" s="112"/>
       <c r="B137" s="40"/>
-      <c r="C137" s="159"/>
+      <c r="C137" s="160"/>
       <c r="D137" s="11" t="s">
         <v>951</v>
       </c>
@@ -33383,7 +33397,7 @@
     <row r="138" customHeight="1" spans="1:5">
       <c r="A138" s="112"/>
       <c r="B138" s="40"/>
-      <c r="C138" s="160"/>
+      <c r="C138" s="161"/>
       <c r="D138" s="11" t="s">
         <v>953</v>
       </c>
@@ -33394,7 +33408,7 @@
     <row r="139" customHeight="1" spans="1:5">
       <c r="A139" s="112"/>
       <c r="B139" s="40"/>
-      <c r="C139" s="158" t="s">
+      <c r="C139" s="159" t="s">
         <v>955</v>
       </c>
       <c r="D139" s="11" t="s">
@@ -33407,7 +33421,7 @@
     <row r="140" customHeight="1" spans="1:5">
       <c r="A140" s="112"/>
       <c r="B140" s="40"/>
-      <c r="C140" s="160"/>
+      <c r="C140" s="161"/>
       <c r="D140" s="49" t="s">
         <v>958</v>
       </c>
@@ -33416,7 +33430,7 @@
     <row r="141" customHeight="1" spans="1:5">
       <c r="A141" s="112"/>
       <c r="B141" s="40"/>
-      <c r="C141" s="158" t="s">
+      <c r="C141" s="159" t="s">
         <v>959</v>
       </c>
       <c r="D141" s="11" t="s">
@@ -33427,7 +33441,7 @@
     <row r="142" customHeight="1" spans="1:5">
       <c r="A142" s="112"/>
       <c r="B142" s="40"/>
-      <c r="C142" s="160"/>
+      <c r="C142" s="161"/>
       <c r="D142" s="49" t="s">
         <v>961</v>
       </c>
@@ -33436,7 +33450,7 @@
     <row r="143" customHeight="1" spans="1:5">
       <c r="A143" s="112"/>
       <c r="B143" s="40"/>
-      <c r="C143" s="158" t="s">
+      <c r="C143" s="159" t="s">
         <v>962</v>
       </c>
       <c r="D143" s="11" t="s">
@@ -33449,7 +33463,7 @@
     <row r="144" customHeight="1" spans="1:5">
       <c r="A144" s="112"/>
       <c r="B144" s="40"/>
-      <c r="C144" s="159"/>
+      <c r="C144" s="160"/>
       <c r="D144" s="49" t="s">
         <v>965</v>
       </c>
@@ -33458,7 +33472,7 @@
     <row r="145" customHeight="1" spans="1:5">
       <c r="A145" s="112"/>
       <c r="B145" s="40"/>
-      <c r="C145" s="159"/>
+      <c r="C145" s="160"/>
       <c r="D145" s="11" t="s">
         <v>966</v>
       </c>
@@ -33467,7 +33481,7 @@
     <row r="146" customHeight="1" spans="1:5">
       <c r="A146" s="111"/>
       <c r="B146" s="42"/>
-      <c r="C146" s="160"/>
+      <c r="C146" s="161"/>
       <c r="D146" s="11" t="s">
         <v>967</v>
       </c>
@@ -34079,7 +34093,7 @@
     <row r="200" ht="147" customHeight="1" spans="1:5">
       <c r="A200" s="111"/>
       <c r="B200" s="42"/>
-      <c r="C200" s="150" t="s">
+      <c r="C200" s="151" t="s">
         <v>1080</v>
       </c>
       <c r="D200" s="109"/>
@@ -34577,11 +34591,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:E129"/>
   <sheetViews>
-    <sheetView zoomScale="99" zoomScaleNormal="99" topLeftCell="A114" workbookViewId="0">
+    <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
@@ -34630,7 +34644,7 @@
         <v>1139</v>
       </c>
       <c r="D3" s="74"/>
-      <c r="E3" s="147" t="s">
+      <c r="E3" s="148" t="s">
         <v>1140</v>
       </c>
     </row>
@@ -35378,7 +35392,7 @@
       <c r="C66" s="49" t="s">
         <v>1288</v>
       </c>
-      <c r="D66" s="148" t="s">
+      <c r="D66" s="149" t="s">
         <v>1289</v>
       </c>
       <c r="E66" s="49"/>
@@ -35389,7 +35403,7 @@
       <c r="C67" s="49" t="s">
         <v>1290</v>
       </c>
-      <c r="D67" s="148" t="s">
+      <c r="D67" s="149" t="s">
         <v>1291</v>
       </c>
       <c r="E67" s="49"/>
@@ -35542,7 +35556,7 @@
         <v>1324</v>
       </c>
       <c r="D79" s="74"/>
-      <c r="E79" s="151" t="s">
+      <c r="E79" s="152" t="s">
         <v>1325</v>
       </c>
     </row>
@@ -35553,7 +35567,7 @@
         <v>1326</v>
       </c>
       <c r="D80" s="74"/>
-      <c r="E80" s="151"/>
+      <c r="E80" s="152"/>
     </row>
     <row r="81" ht="71" customHeight="1" spans="1:5">
       <c r="A81" s="112"/>
@@ -35562,7 +35576,7 @@
         <v>1327</v>
       </c>
       <c r="D81" s="134"/>
-      <c r="E81" s="151" t="s">
+      <c r="E81" s="152" t="s">
         <v>1328</v>
       </c>
     </row>
@@ -35597,7 +35611,7 @@
         <v>1334</v>
       </c>
       <c r="D84" s="109"/>
-      <c r="E84" s="147" t="s">
+      <c r="E84" s="148" t="s">
         <v>1335</v>
       </c>
     </row>
@@ -35611,7 +35625,7 @@
       <c r="C85" s="49" t="s">
         <v>1338</v>
       </c>
-      <c r="D85" s="149" t="s">
+      <c r="D85" s="150" t="s">
         <v>1339</v>
       </c>
       <c r="E85" s="49"/>
@@ -35620,7 +35634,7 @@
       <c r="A86" s="112"/>
       <c r="B86" s="40"/>
       <c r="C86" s="49"/>
-      <c r="D86" s="149" t="s">
+      <c r="D86" s="150" t="s">
         <v>1340</v>
       </c>
       <c r="E86" s="49"/>
@@ -35629,7 +35643,7 @@
       <c r="A87" s="112"/>
       <c r="B87" s="40"/>
       <c r="C87" s="49"/>
-      <c r="D87" s="149" t="s">
+      <c r="D87" s="150" t="s">
         <v>1341</v>
       </c>
       <c r="E87" s="49"/>
@@ -35638,7 +35652,7 @@
       <c r="A88" s="111"/>
       <c r="B88" s="42"/>
       <c r="C88" s="49"/>
-      <c r="D88" s="149" t="s">
+      <c r="D88" s="150" t="s">
         <v>1342</v>
       </c>
       <c r="E88" s="49"/>
@@ -35976,7 +35990,7 @@
     <row r="115" customHeight="1" spans="1:5">
       <c r="A115" s="112"/>
       <c r="B115" s="40"/>
-      <c r="C115" s="150" t="s">
+      <c r="C115" s="151" t="s">
         <v>1417</v>
       </c>
       <c r="D115" s="143"/>
@@ -35987,7 +36001,7 @@
     <row r="116" customHeight="1" spans="1:5">
       <c r="A116" s="111"/>
       <c r="B116" s="42"/>
-      <c r="C116" s="150" t="s">
+      <c r="C116" s="151" t="s">
         <v>1419</v>
       </c>
       <c r="D116" s="143"/>
@@ -36152,7 +36166,7 @@
       <c r="B129" s="49" t="s">
         <v>1454</v>
       </c>
-      <c r="C129" s="150" t="s">
+      <c r="C129" s="151" t="s">
         <v>1455</v>
       </c>
       <c r="D129" s="109"/>
@@ -36300,14 +36314,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:E259"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A199" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A252" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A210" sqref="A210:A222"/>
+      <selection pane="bottomLeft" activeCell="D252" sqref="D252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="4"/>
@@ -39169,7 +39183,7 @@
       <c r="C252" s="49" t="s">
         <v>1983</v>
       </c>
-      <c r="D252" s="22" t="s">
+      <c r="D252" s="144" t="s">
         <v>1984</v>
       </c>
       <c r="E252" s="49"/>
@@ -39205,10 +39219,10 @@
       <c r="B255" s="44" t="s">
         <v>1990</v>
       </c>
-      <c r="C255" s="144" t="s">
+      <c r="C255" s="145" t="s">
         <v>1991</v>
       </c>
-      <c r="D255" s="145" t="s">
+      <c r="D255" s="146" t="s">
         <v>1992</v>
       </c>
       <c r="E255" s="124" t="s">
@@ -39218,10 +39232,10 @@
     <row r="256" customHeight="1" spans="1:5">
       <c r="A256" s="112"/>
       <c r="B256" s="40"/>
-      <c r="C256" s="144" t="s">
+      <c r="C256" s="145" t="s">
         <v>1994</v>
       </c>
-      <c r="D256" s="146" t="s">
+      <c r="D256" s="147" t="s">
         <v>1995</v>
       </c>
       <c r="E256" s="124" t="s">
@@ -39507,14 +39521,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:E347"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C45" sqref="C45:D45"/>
+      <selection pane="bottomLeft" activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="4"/>
@@ -43846,7 +43860,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:F103"/>
   <sheetViews>
@@ -45333,7 +45347,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:J172"/>
   <sheetViews>

</xml_diff>